<commit_message>
Fixed bed times after midnight. Added conditional option to select report figures y-axis format
</commit_message>
<xml_diff>
--- a/Report templates/Report template_somfit_CG.xlsx
+++ b/Report templates/Report template_somfit_CG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s4548745\Desktop\ACU\ACU_SPRINT_Sleep\Report templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B1379B-6DBA-43DC-B52A-322C0F0B748F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0233ACFD-7D18-4230-A108-C73F522A4DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{76E57436-7828-490E-9B39-280DBAE6617A}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{76E57436-7828-490E-9B39-280DBAE6617A}"/>
   </bookViews>
   <sheets>
     <sheet name="Report - Short" sheetId="6" r:id="rId1"/>
@@ -296,7 +296,7 @@
     <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="167" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,6 +379,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11.5"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -406,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -475,6 +481,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2570,15 +2579,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
+      <xdr:colOff>55246</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>630555</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:colOff>668021</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>154305</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2670,13 +2679,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>811533</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>163871</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2731,13 +2740,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>262890</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>563794</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2799,13 +2808,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1018226</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>47627</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1313541</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>47627</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2907,14 +2916,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>739020</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:colOff>697110</xdr:colOff>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>171045</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2945,15 +2954,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
+      <xdr:colOff>592455</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>36195</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>449539</xdr:colOff>
+      <xdr:colOff>720684</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>213120</xdr:rowOff>
+      <xdr:rowOff>211215</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2981,8 +2990,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5707380" y="274320"/>
-          <a:ext cx="853399" cy="396000"/>
+          <a:off x="5650230" y="36195"/>
+          <a:ext cx="861654" cy="403620"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3004,14 +3013,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:colOff>5715</xdr:colOff>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>700920</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:colOff>699015</xdr:colOff>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>169140</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3339,18 +3348,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF86B646-CAF6-473E-9E5F-FA6562A84B8A}">
-  <dimension ref="A1:J254"/>
+  <dimension ref="A1:J253"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="11" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="9" width="11" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="10.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="9" width="10.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.109375" style="1"/>
     <col min="11" max="16384" width="9.109375" style="1" collapsed="1"/>
   </cols>
@@ -3400,7 +3408,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="10" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" s="10" customFormat="1" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D8" s="11" t="s">
         <v>4</v>
       </c>
@@ -3414,7 +3422,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
     </row>
-    <row r="9" spans="1:9" s="10" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" s="10" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -3434,7 +3442,7 @@
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" spans="1:9" s="10" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="10" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>8</v>
       </c>
@@ -3454,7 +3462,7 @@
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" spans="1:9" s="10" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" s="10" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
@@ -3473,8 +3481,8 @@
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
     </row>
-    <row r="12" spans="1:9" s="10" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:9" s="10" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
         <v>63</v>
       </c>
       <c r="D12" s="20">
@@ -3493,8 +3501,8 @@
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
     </row>
-    <row r="13" spans="1:9" s="10" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:9" s="10" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
         <v>64</v>
       </c>
       <c r="D13" s="20">
@@ -3512,8 +3520,8 @@
       <c r="G13" s="20"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" s="10" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+    <row r="14" spans="1:9" s="10" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
         <v>65</v>
       </c>
       <c r="D14" s="20">
@@ -3532,7 +3540,7 @@
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
     </row>
-    <row r="15" spans="1:9" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" s="4" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
@@ -3553,7 +3561,7 @@
       <c r="H15" s="20"/>
       <c r="I15" s="20"/>
     </row>
-    <row r="16" spans="1:9" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="4" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="14"/>
       <c r="D16" s="11" t="s">
@@ -3575,7 +3583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="10" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" s="10" customFormat="1" ht="24.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -3590,8 +3598,8 @@
       <c r="H17" s="31"/>
       <c r="I17" s="31"/>
     </row>
-    <row r="18" spans="1:9" s="10" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+    <row r="18" spans="1:9" s="10" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
         <v>60</v>
       </c>
       <c r="B18" s="13"/>
@@ -3620,8 +3628,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="10" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:9" s="10" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
         <v>61</v>
       </c>
       <c r="B19" s="13"/>
@@ -3650,8 +3658,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="10" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+    <row r="20" spans="1:9" s="10" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
         <v>62</v>
       </c>
       <c r="B20" s="13"/>
@@ -3680,8 +3688,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+    <row r="21" spans="1:9" s="4" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="14"/>
@@ -3710,8 +3718,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:9" s="4" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" s="4" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:9" s="4" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="D23" s="15" t="s">
         <v>11</v>
@@ -3774,21 +3782,31 @@
     <row r="58" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="26"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
+    </row>
     <row r="62" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="26"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="26"/>
-      <c r="E62" s="26"/>
-      <c r="F62" s="26"/>
-      <c r="G62" s="26"/>
-      <c r="H62" s="26"/>
-      <c r="I62" s="26"/>
+      <c r="A62" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B62" s="32"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="32"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="32"/>
+      <c r="G62" s="32"/>
+      <c r="H62" s="32"/>
+      <c r="I62" s="32"/>
     </row>
     <row r="63" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="32" t="s">
-        <v>18</v>
-      </c>
+      <c r="A63" s="32"/>
       <c r="B63" s="32"/>
       <c r="C63" s="32"/>
       <c r="D63" s="32"/>
@@ -3809,18 +3827,15 @@
       <c r="H64" s="32"/>
       <c r="I64" s="32"/>
     </row>
-    <row r="65" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="32"/>
-      <c r="B65" s="32"/>
-      <c r="C65" s="32"/>
-      <c r="D65" s="32"/>
-      <c r="E65" s="32"/>
-      <c r="F65" s="32"/>
-      <c r="G65" s="32"/>
-      <c r="H65" s="32"/>
-      <c r="I65" s="32"/>
-    </row>
-    <row r="66" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="25"/>
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="25"/>
+    </row>
+    <row r="66" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="25"/>
       <c r="B66" s="25"/>
       <c r="C66" s="25"/>
@@ -3828,7 +3843,7 @@
       <c r="E66" s="25"/>
       <c r="F66" s="25"/>
     </row>
-    <row r="67" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="25"/>
       <c r="B67" s="25"/>
       <c r="C67" s="25"/>
@@ -3836,36 +3851,36 @@
       <c r="E67" s="25"/>
       <c r="F67" s="25"/>
     </row>
-    <row r="68" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="25"/>
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="25"/>
-    </row>
-    <row r="69" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:9" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="12"/>
-    </row>
-    <row r="86" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="17"/>
+    <row r="84" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="12"/>
+    </row>
+    <row r="85" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="17"/>
+    </row>
+    <row r="87" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="29"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="29"/>
+      <c r="D87" s="29"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="29"/>
     </row>
     <row r="88" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="29"/>
@@ -3899,14 +3914,7 @@
       <c r="E91" s="29"/>
       <c r="F91" s="29"/>
     </row>
-    <row r="92" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="29"/>
-      <c r="B92" s="29"/>
-      <c r="C92" s="29"/>
-      <c r="D92" s="29"/>
-      <c r="E92" s="29"/>
-      <c r="F92" s="29"/>
-    </row>
+    <row r="92" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="93" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="94" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="95" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3980,15 +3988,22 @@
     <row r="163" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="164" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="165" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" spans="1:6" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="12"/>
-      <c r="B168" s="12"/>
-      <c r="C168" s="12"/>
-      <c r="D168" s="12"/>
-      <c r="E168" s="12"/>
-      <c r="F168" s="12"/>
+    <row r="166" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A167" s="12"/>
+      <c r="B167" s="12"/>
+      <c r="C167" s="12"/>
+      <c r="D167" s="12"/>
+      <c r="E167" s="12"/>
+      <c r="F167" s="12"/>
+    </row>
+    <row r="168" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="18"/>
+      <c r="B168" s="18"/>
+      <c r="C168" s="18"/>
+      <c r="D168" s="18"/>
+      <c r="E168" s="18"/>
+      <c r="F168" s="18"/>
     </row>
     <row r="169" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="18"/>
@@ -4094,7 +4109,7 @@
       <c r="E181" s="18"/>
       <c r="F181" s="18"/>
     </row>
-    <row r="182" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:6" s="4" customFormat="1" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="18"/>
       <c r="B182" s="18"/>
       <c r="C182" s="18"/>
@@ -4102,7 +4117,7 @@
       <c r="E182" s="18"/>
       <c r="F182" s="18"/>
     </row>
-    <row r="183" spans="1:6" s="4" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="18"/>
       <c r="B183" s="18"/>
       <c r="C183" s="18"/>
@@ -4118,7 +4133,7 @@
       <c r="E184" s="18"/>
       <c r="F184" s="18"/>
     </row>
-    <row r="185" spans="1:6" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A185" s="18"/>
       <c r="B185" s="18"/>
       <c r="C185" s="18"/>
@@ -4126,7 +4141,7 @@
       <c r="E185" s="18"/>
       <c r="F185" s="18"/>
     </row>
-    <row r="186" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:6" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="18"/>
       <c r="B186" s="18"/>
       <c r="C186" s="18"/>
@@ -4159,23 +4174,23 @@
       <c r="F189" s="18"/>
     </row>
     <row r="190" spans="1:6" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A190" s="18"/>
-      <c r="B190" s="18"/>
-      <c r="C190" s="18"/>
-      <c r="D190" s="18"/>
-      <c r="E190" s="18"/>
-      <c r="F190" s="18"/>
-    </row>
-    <row r="191" spans="1:6" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="1"/>
-      <c r="B191" s="1"/>
-      <c r="C191" s="1"/>
-      <c r="D191" s="1"/>
-      <c r="E191" s="1"/>
-      <c r="F191" s="1"/>
-    </row>
+      <c r="A190" s="1"/>
+      <c r="B190" s="1"/>
+      <c r="C190" s="1"/>
+      <c r="D190" s="1"/>
+      <c r="E190" s="1"/>
+      <c r="F190" s="1"/>
+    </row>
+    <row r="191" spans="1:6" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="192" spans="1:6" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" spans="1:6" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" spans="1:6" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="1"/>
+      <c r="B193" s="1"/>
+      <c r="C193" s="1"/>
+      <c r="D193" s="1"/>
+      <c r="E193" s="1"/>
+      <c r="F193" s="1"/>
+    </row>
     <row r="194" spans="1:6" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1"/>
       <c r="B194" s="1"/>
@@ -4656,33 +4671,25 @@
       <c r="E253" s="1"/>
       <c r="F253" s="1"/>
     </row>
-    <row r="254" spans="1:6" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A254" s="1"/>
-      <c r="B254" s="1"/>
-      <c r="C254" s="1"/>
-      <c r="D254" s="1"/>
-      <c r="E254" s="1"/>
-      <c r="F254" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A92:F92"/>
+    <mergeCell ref="A91:F91"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="G17:I17"/>
+    <mergeCell ref="A87:F87"/>
     <mergeCell ref="A88:F88"/>
     <mergeCell ref="A89:F89"/>
     <mergeCell ref="A90:F90"/>
-    <mergeCell ref="A91:F91"/>
-    <mergeCell ref="A63:I65"/>
+    <mergeCell ref="A62:I64"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.55118110236220474" bottom="0.55118110236220474" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="93" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="4" manualBreakCount="4">
-    <brk id="39" max="9" man="1"/>
-    <brk id="92" max="16383" man="1"/>
-    <brk id="96" max="16383" man="1"/>
-    <brk id="191" max="16383" man="1"/>
+    <brk id="38" max="9" man="1"/>
+    <brk id="91" max="16383" man="1"/>
+    <brk id="95" max="16383" man="1"/>
+    <brk id="190" max="16383" man="1"/>
   </rowBreaks>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -4694,14 +4701,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.88671875" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="8.77734375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="7" width="8.77734375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -4802,17 +4808,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="16.33203125" customWidth="1"/>
     <col min="12" max="15" width="13.33203125" customWidth="1"/>
   </cols>
@@ -5966,7 +5972,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" style="22" customWidth="1"/>
     <col min="2" max="3" width="12" style="23" customWidth="1"/>
@@ -5978,12 +5984,12 @@
     <col min="19" max="35" width="12" customWidth="1"/>
     <col min="36" max="36" width="14" customWidth="1"/>
     <col min="37" max="40" width="12" customWidth="1"/>
-    <col min="41" max="42" width="13.5546875" customWidth="1"/>
+    <col min="41" max="42" width="13.44140625" customWidth="1"/>
     <col min="43" max="43" width="12" customWidth="1"/>
     <col min="44" max="49" width="14" customWidth="1"/>
     <col min="50" max="50" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" s="28" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>